<commit_message>
update with new information
</commit_message>
<xml_diff>
--- a/markdown_generator/publications.xlsx
+++ b/markdown_generator/publications.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotty/Github/scottyih.github.io/markdown_generator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottyih/GitHub/scottyih.github.io/markdown_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56096E3B-5D28-E046-BA61-4E1C9EA69ED7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103438DE-1354-114E-8066-F548C0CA0DF1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="860" yWindow="880" windowWidth="30000" windowHeight="18220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publications.raw" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="698">
   <si>
     <t>Po-Sen Huang, Chenglong Wang, Rishabh Singh, Wen-tau Yih and Xiaodong He</t>
   </si>
@@ -3484,6 +3484,44 @@
   month={May},
   address={New Orleans, Louisiana}
 }</t>
+  </si>
+  <si>
+    <t>Be Consistent! Improving Procedural Text Comprehension using Label Consistency</t>
+  </si>
+  <si>
+    <t>NAACL-HLT-2019</t>
+  </si>
+  <si>
+    <t>Xinya Du, Bhavana Dalvi, Niket Tandon, Antoine Bosselut, Wen-tau Yih, Peter Clark and Claire Cardie</t>
+  </si>
+  <si>
+    <t>naacl19_ai2_be_consistent.pdf</t>
+  </si>
+  <si>
+    <t>Our goal is procedural text comprehension,
+namely tracking how the properties of entities
+(e.g., their location) change with time given a
+procedural text (e.g., a paragraph about photosynthesis, a recipe). This task is challenging as the world is changing throughout the
+text, and despite recent advances, current systems still struggle with this task. Our approach
+is to leverage the fact that, for many procedural texts, multiple independent descriptions
+are readily available, and that predictions from
+them should be consistent (label consistency).
+We present a new learning framework that
+leverages label consistency during training, allowing consistency bias to be built into the
+model. Evaluation on a standard benchmark
+dataset for procedural text, ProPara (Dalvi
+et al., 2018), shows that our approach significantly improves prediction performance (F1)
+over prior state-of-the-art systems.</t>
+  </si>
+  <si>
+    <t>@InProceedings{dalvi-EtAl:2018:N18-1,
+  author    = {Xinya Du and Bhavana Dalvi and Niket Tandon and Antoine Bosselut and Yih, Wen-tau and Peter Clark and Claire Cardie},
+  title     = {Be Consistent! Improving Procedural Text Comprehension using Label Consistency},
+  booktitle = {Proceedings of the 2019 Conference of the North American Chapter of the Association for Computational Linguistics: Human Language Technologies, Volume 1 (Long Papers)},
+  month     = {June},
+  year      = {2019},
+  address   = {Minneapolis, USA},
+  publisher = {Association for Computational Linguistics} }</t>
   </si>
 </sst>
 </file>
@@ -5639,11 +5677,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M74"/>
+  <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5704,1735 +5742,1732 @@
         <v>389</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" ht="289" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="5" customFormat="1" ht="340" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
+        <v>43619</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>692</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>694</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>696</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>697</v>
+      </c>
+      <c r="G2" s="5">
+        <v>74</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="5" customFormat="1" ht="289" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
         <v>43591</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B3" s="5" t="s">
         <v>686</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>690</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>687</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>688</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F3" s="15" t="s">
         <v>691</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G3" s="5">
         <v>73</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>684</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+    <row r="4" spans="1:13" s="5" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
         <v>43492</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>677</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>678</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>679</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>689</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F4" s="15" t="s">
         <v>683</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G4" s="5">
         <v>72</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" ht="306" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
-        <v>43404</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>398</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>631</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>461</v>
-      </c>
-      <c r="G4">
-        <v>71</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="5" customFormat="1" ht="372" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="5" customFormat="1" ht="306" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>43404</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>393</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G5">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>681</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="5" customFormat="1" ht="404" x14ac:dyDescent="0.2">
+        <v>454</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="5" customFormat="1" ht="372" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>43404</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>673</v>
+        <v>396</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>394</v>
+      <c r="D6" s="5" t="s">
+        <v>395</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>459</v>
+        <v>632</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>676</v>
+        <v>462</v>
       </c>
       <c r="G6">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="5" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
+        <v>456</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>681</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="5" customFormat="1" ht="404" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>43404</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>392</v>
+        <v>673</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>459</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>676</v>
+      </c>
+      <c r="G7">
+        <v>69</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="5" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>43404</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>674</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E8" s="13" t="s">
         <v>460</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F8" s="15" t="s">
         <v>675</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <v>68</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H8" s="14" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="259" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>43253</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>294</v>
-      </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>414</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>415</v>
-      </c>
-      <c r="G8">
-        <v>67</v>
-      </c>
-      <c r="H8" t="s">
-        <v>413</v>
-      </c>
-      <c r="L8" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="291" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="259" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>43253</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>294</v>
       </c>
       <c r="D9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="G9">
+        <v>67</v>
+      </c>
+      <c r="H9" t="s">
+        <v>413</v>
+      </c>
+      <c r="L9" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="291" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>43253</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>294</v>
+      </c>
+      <c r="D10" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F10" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="G9">
+      <c r="G10">
         <v>66</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>416</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K10" t="s">
         <v>417</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L10" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="272" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+    <row r="11" spans="1:13" ht="272" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
         <v>43133</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>295</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E11" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F11" s="8" t="s">
         <v>423</v>
       </c>
-      <c r="G10">
+      <c r="G11">
         <v>65</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H11" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="340" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+    <row r="12" spans="1:13" ht="340" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
         <v>42985</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>296</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>425</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="G11">
+      <c r="G12">
         <v>64</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H12" t="s">
         <v>426</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J12" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="345" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
-        <v>42946</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>297</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>403</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="G12">
-        <v>63</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>400</v>
-      </c>
-      <c r="I12" t="s">
-        <v>406</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>404</v>
-      </c>
-      <c r="L12" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="404" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="345" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>42946</v>
       </c>
       <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>297</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="G13">
+        <v>63</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="I13" t="s">
+        <v>406</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="L13" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="404" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>42946</v>
+      </c>
+      <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>298</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>428</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>62</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H14" s="11" t="s">
         <v>427</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J14" t="s">
         <v>452</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K14" t="s">
         <v>407</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L14" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="306" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+    <row r="15" spans="1:13" ht="306" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
         <v>42675</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>299</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E15" s="8" t="s">
         <v>432</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F15" s="8" t="s">
         <v>431</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <v>61</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H15" t="s">
         <v>430</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J15" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="372" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>42589</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>300</v>
-      </c>
-      <c r="D15" t="s">
-        <v>358</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>439</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>438</v>
-      </c>
-      <c r="G15">
-        <v>60</v>
-      </c>
-      <c r="H15" t="s">
-        <v>437</v>
-      </c>
-      <c r="J15" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="272" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="372" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>42589</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
         <v>300</v>
       </c>
       <c r="D16" t="s">
+        <v>358</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="G16">
+        <v>60</v>
+      </c>
+      <c r="H16" t="s">
+        <v>437</v>
+      </c>
+      <c r="J16" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="272" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>42589</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>300</v>
+      </c>
+      <c r="D17" t="s">
         <v>319</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>442</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F17" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>59</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H17" t="s">
         <v>440</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I17" t="s">
         <v>444</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="K17" s="7" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="356" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+    <row r="18" spans="1:13" ht="356" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
         <v>42492</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>38</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>301</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>320</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>446</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F18" s="8" t="s">
         <v>447</v>
       </c>
-      <c r="G17">
+      <c r="G18">
         <v>58</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H18" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+    <row r="19" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
         <v>42471</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>42</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>305</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>321</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E19" s="8" t="s">
         <v>449</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F19" s="8" t="s">
         <v>450</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <v>57</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H19" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="388" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+    <row r="20" spans="1:13" ht="388" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
         <v>42264</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>47</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>303</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>322</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E20" s="10" t="s">
         <v>464</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F20" s="8" t="s">
         <v>463</v>
       </c>
-      <c r="G19">
+      <c r="G20">
         <v>56</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H20" t="s">
         <v>465</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I20" t="s">
         <v>468</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K20" t="s">
         <v>466</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L20" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="323" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+    <row r="21" spans="1:13" ht="323" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
         <v>42213</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>50</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>304</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>323</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E21" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F21" s="8" t="s">
         <v>471</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <v>55</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H21" t="s">
         <v>473</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I21" t="s">
         <v>469</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J21" t="s">
         <v>451</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L21" t="s">
         <v>470</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M21" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="388" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+    <row r="22" spans="1:13" ht="388" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
         <v>42125</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>57</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>306</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>324</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E22" s="10" t="s">
         <v>475</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F22" s="8" t="s">
         <v>476</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <v>54</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H22" t="s">
         <v>474</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I22" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="404" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
-        <v>42144</v>
-      </c>
-      <c r="B22" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" t="s">
-        <v>302</v>
-      </c>
-      <c r="D22" t="s">
-        <v>325</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>480</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>482</v>
-      </c>
-      <c r="G22">
-        <v>53</v>
-      </c>
-      <c r="H22" t="s">
-        <v>481</v>
-      </c>
-      <c r="I22" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="404" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>42144</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
         <v>302</v>
       </c>
       <c r="D23" t="s">
+        <v>325</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="G23">
+        <v>53</v>
+      </c>
+      <c r="H23" t="s">
+        <v>481</v>
+      </c>
+      <c r="I23" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>42144</v>
+      </c>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" t="s">
+        <v>302</v>
+      </c>
+      <c r="D24" t="s">
         <v>326</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E24" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F24" s="8" t="s">
         <v>483</v>
       </c>
-      <c r="G23">
+      <c r="G24">
         <v>52</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H24" t="s">
         <v>485</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I24" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="289" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
+    <row r="25" spans="1:13" ht="289" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
         <v>42244</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>66</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>307</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>327</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E25" s="10" t="s">
         <v>488</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F25" s="8" t="s">
         <v>487</v>
       </c>
-      <c r="G24">
+      <c r="G25">
         <v>51</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H25" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+    <row r="26" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
         <v>41983</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>73</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>308</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>328</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E26" s="10" t="s">
         <v>490</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F26" s="8" t="s">
         <v>491</v>
       </c>
-      <c r="G25">
+      <c r="G26">
         <v>50</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H26" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="404" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+    <row r="27" spans="1:13" ht="404" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
         <v>41937</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>81</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>309</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>329</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E27" s="10" t="s">
         <v>493</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F27" s="8" t="s">
         <v>494</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <v>49</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H27" t="s">
         <v>492</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I27" t="s">
         <v>495</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J27" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="340" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
-        <v>41813</v>
-      </c>
-      <c r="B27" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" t="s">
-        <v>388</v>
-      </c>
-      <c r="D27" t="s">
-        <v>330</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>497</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>498</v>
-      </c>
-      <c r="G27">
-        <v>48</v>
-      </c>
-      <c r="H27" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="306" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="340" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>41813</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s">
         <v>388</v>
       </c>
       <c r="D28" t="s">
+        <v>330</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="G28">
+        <v>48</v>
+      </c>
+      <c r="H28" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="306" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>41813</v>
+      </c>
+      <c r="B29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" t="s">
+        <v>388</v>
+      </c>
+      <c r="D29" t="s">
         <v>331</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E29" s="8" t="s">
         <v>500</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F29" s="8" t="s">
         <v>501</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <v>47</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H29" t="s">
         <v>499</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I29" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="221" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
-        <v>41565</v>
-      </c>
-      <c r="B29" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" t="s">
-        <v>399</v>
-      </c>
-      <c r="D29" t="s">
-        <v>332</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>504</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>505</v>
-      </c>
-      <c r="G29">
-        <v>46</v>
-      </c>
-      <c r="H29" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="323" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>41565</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C30" t="s">
         <v>399</v>
       </c>
       <c r="D30" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="G30">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H30" t="s">
-        <v>509</v>
-      </c>
-      <c r="I30" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="323" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
+        <v>41565</v>
+      </c>
+      <c r="B31" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" t="s">
+        <v>399</v>
+      </c>
+      <c r="D31" t="s">
+        <v>333</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>507</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="G31">
+        <v>45</v>
+      </c>
+      <c r="H31" t="s">
+        <v>509</v>
+      </c>
+      <c r="I31" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="323" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
         <v>41490</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>101</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>503</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D32" t="s">
         <v>334</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F32" s="8" t="s">
         <v>512</v>
       </c>
-      <c r="G31">
+      <c r="G32">
         <v>44</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H32" t="s">
         <v>513</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I32" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
-        <v>41421</v>
-      </c>
-      <c r="B32" t="s">
-        <v>105</v>
-      </c>
-      <c r="C32" t="s">
-        <v>310</v>
-      </c>
-      <c r="D32" t="s">
-        <v>335</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>518</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>517</v>
-      </c>
-      <c r="G32">
-        <v>43</v>
-      </c>
-      <c r="H32" t="s">
-        <v>516</v>
-      </c>
-      <c r="K32" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="238" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>41421</v>
       </c>
       <c r="B33" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C33" t="s">
         <v>310</v>
       </c>
       <c r="D33" t="s">
+        <v>335</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>518</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>517</v>
+      </c>
+      <c r="G33">
+        <v>43</v>
+      </c>
+      <c r="H33" t="s">
+        <v>516</v>
+      </c>
+      <c r="K33" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="238" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>41421</v>
+      </c>
+      <c r="B34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" t="s">
+        <v>310</v>
+      </c>
+      <c r="D34" t="s">
         <v>336</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E34" s="10" t="s">
         <v>520</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F34" s="8" t="s">
         <v>521</v>
       </c>
-      <c r="G33">
+      <c r="G34">
         <v>42</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H34" t="s">
         <v>519</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I34" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="356" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
+    <row r="35" spans="1:13" ht="356" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
         <v>41565</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>111</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>298</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>110</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E35" s="10" t="s">
         <v>524</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F35" s="8" t="s">
         <v>526</v>
       </c>
-      <c r="G34">
+      <c r="G35">
         <v>41</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H35" t="s">
         <v>523</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I35" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="372" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
+    <row r="36" spans="1:13" ht="372" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
         <v>41102</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>116</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>311</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D36" t="s">
         <v>337</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E36" s="10" t="s">
         <v>528</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F36" s="8" t="s">
         <v>527</v>
       </c>
-      <c r="G35">
+      <c r="G36">
         <v>40</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H36" t="s">
         <v>529</v>
       </c>
-      <c r="I35" s="7" t="s">
+      <c r="I36" s="7" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="221" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
-        <v>41062</v>
-      </c>
-      <c r="B36" t="s">
-        <v>120</v>
-      </c>
-      <c r="C36" t="s">
-        <v>312</v>
-      </c>
-      <c r="D36" t="s">
-        <v>119</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>532</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>533</v>
-      </c>
-      <c r="G36">
-        <v>39</v>
-      </c>
-      <c r="H36" t="s">
-        <v>531</v>
-      </c>
-      <c r="I36" s="7" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="255" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>41062</v>
       </c>
       <c r="B37" t="s">
-        <v>313</v>
+        <v>120</v>
       </c>
       <c r="C37" t="s">
         <v>312</v>
       </c>
       <c r="D37" t="s">
+        <v>119</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="G37">
+        <v>39</v>
+      </c>
+      <c r="H37" t="s">
+        <v>531</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="255" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>41062</v>
+      </c>
+      <c r="B38" t="s">
+        <v>313</v>
+      </c>
+      <c r="C38" t="s">
+        <v>312</v>
+      </c>
+      <c r="D38" t="s">
         <v>338</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E38" s="10" t="s">
         <v>535</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F38" s="8" t="s">
         <v>536</v>
       </c>
-      <c r="G37">
+      <c r="G38">
         <v>38</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H38" t="s">
         <v>537</v>
       </c>
-      <c r="L37" t="s">
+      <c r="L38" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
+    <row r="39" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
         <v>40748</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>129</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>314</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>339</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E39" s="8" t="s">
         <v>540</v>
       </c>
-      <c r="F38" s="8" t="s">
+      <c r="F39" s="8" t="s">
         <v>539</v>
       </c>
-      <c r="G38">
+      <c r="G39">
         <v>37</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H39" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="306" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
+    <row r="40" spans="1:13" ht="306" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
         <v>40740</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>134</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>315</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>133</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E40" s="10" t="s">
         <v>543</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F40" s="8" t="s">
         <v>542</v>
       </c>
-      <c r="G39">
+      <c r="G40">
         <v>36</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H40" t="s">
         <v>544</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I40" t="s">
         <v>549</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J40" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="289" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
+    <row r="41" spans="1:13" ht="289" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
         <v>40707</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>138</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>316</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>340</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E41" s="10" t="s">
         <v>547</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="F41" s="8" t="s">
         <v>545</v>
       </c>
-      <c r="G40">
+      <c r="G41">
         <v>35</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H41" t="s">
         <v>546</v>
       </c>
-      <c r="I40" s="7" t="s">
+      <c r="I41" s="7" t="s">
         <v>548</v>
       </c>
-      <c r="M40" t="s">
+      <c r="M41" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="323" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
+    <row r="42" spans="1:13" ht="323" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
         <v>40522</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>142</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>317</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>141</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E42" s="10" t="s">
         <v>551</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F42" s="8" t="s">
         <v>550</v>
       </c>
-      <c r="G41">
+      <c r="G42">
         <v>34</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H42" t="s">
         <v>552</v>
       </c>
-      <c r="I41" s="7" t="s">
+      <c r="I42" s="7" t="s">
         <v>553</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
-        <v>40460</v>
-      </c>
-      <c r="B42" t="s">
-        <v>150</v>
-      </c>
-      <c r="C42" t="s">
-        <v>318</v>
-      </c>
-      <c r="D42" t="s">
-        <v>341</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>555</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>554</v>
-      </c>
-      <c r="G42">
-        <v>33</v>
-      </c>
-      <c r="H42" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
+        <v>40460</v>
+      </c>
+      <c r="B43" t="s">
+        <v>150</v>
+      </c>
+      <c r="C43" t="s">
+        <v>318</v>
+      </c>
+      <c r="D43" t="s">
+        <v>341</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>555</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>554</v>
+      </c>
+      <c r="G43">
+        <v>33</v>
+      </c>
+      <c r="H43" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
         <v>40378</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>154</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>387</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>342</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E44" s="10" t="s">
         <v>558</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="F44" s="8" t="s">
         <v>557</v>
       </c>
-      <c r="G43">
+      <c r="G44">
         <v>32</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H44" t="s">
         <v>559</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I44" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="388" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
+    <row r="45" spans="1:13" ht="388" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
         <v>40032</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>359</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>360</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>292</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E45" s="10" t="s">
         <v>562</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="F45" s="8" t="s">
         <v>561</v>
       </c>
-      <c r="G44">
+      <c r="G45">
         <v>31</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H45" t="s">
         <v>563</v>
       </c>
-      <c r="I44" s="7" t="s">
+      <c r="I45" s="7" t="s">
         <v>564</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A45" s="3">
-        <v>40011</v>
-      </c>
-      <c r="B45" t="s">
-        <v>161</v>
-      </c>
-      <c r="C45" t="s">
-        <v>361</v>
-      </c>
-      <c r="D45" t="s">
-        <v>160</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>575</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="G45">
-        <v>30</v>
-      </c>
-      <c r="H45" t="s">
-        <v>574</v>
-      </c>
-      <c r="I45" s="7" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
-        <v>39684</v>
+        <v>40011</v>
       </c>
       <c r="B46" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C46" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D46" t="s">
-        <v>343</v>
+        <v>160</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="G46">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H46" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="306" x14ac:dyDescent="0.2">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>39684</v>
       </c>
       <c r="B47" t="s">
+        <v>166</v>
+      </c>
+      <c r="C47" t="s">
+        <v>362</v>
+      </c>
+      <c r="D47" t="s">
+        <v>343</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>579</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="G47">
+        <v>29</v>
+      </c>
+      <c r="H47" t="s">
+        <v>578</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="306" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>39684</v>
+      </c>
+      <c r="B48" t="s">
         <v>170</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>363</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D48" t="s">
         <v>169</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="E48" s="8" t="s">
         <v>434</v>
       </c>
-      <c r="F47" s="8" t="s">
+      <c r="F48" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="G47">
+      <c r="G48">
         <v>28</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H48" t="s">
         <v>433</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I48" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="238" x14ac:dyDescent="0.2">
-      <c r="A48" s="3">
+    <row r="49" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+      <c r="A49" s="3">
         <v>39681</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>174</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>364</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>344</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E49" s="10" t="s">
         <v>566</v>
       </c>
-      <c r="F48" s="8" t="s">
+      <c r="F49" s="8" t="s">
         <v>567</v>
       </c>
-      <c r="G48">
+      <c r="G49">
         <v>27</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H49" t="s">
         <v>565</v>
       </c>
-      <c r="I48" s="7" t="s">
+      <c r="I49" s="7" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="356" x14ac:dyDescent="0.2">
-      <c r="A49" s="3">
+    <row r="50" spans="1:9" ht="356" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
         <v>39173</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>178</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>365</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>345</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E50" s="8" t="s">
         <v>570</v>
       </c>
-      <c r="F49" s="8" t="s">
+      <c r="F50" s="8" t="s">
         <v>571</v>
       </c>
-      <c r="G49">
+      <c r="G50">
         <v>26</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H50" t="s">
         <v>569</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A50" s="3">
-        <v>39416</v>
-      </c>
-      <c r="B50" t="s">
-        <v>185</v>
-      </c>
-      <c r="C50" t="s">
-        <v>366</v>
-      </c>
-      <c r="D50" t="s">
-        <v>184</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>573</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>591</v>
-      </c>
-      <c r="G50">
-        <v>25</v>
-      </c>
-      <c r="H50" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
+        <v>39416</v>
+      </c>
+      <c r="B51" t="s">
+        <v>185</v>
+      </c>
+      <c r="C51" t="s">
+        <v>366</v>
+      </c>
+      <c r="D51" t="s">
+        <v>184</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>573</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>591</v>
+      </c>
+      <c r="G51">
+        <v>25</v>
+      </c>
+      <c r="H51" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
         <v>39345</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>190</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>367</v>
-      </c>
-      <c r="D51" t="s">
-        <v>189</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>582</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>583</v>
-      </c>
-      <c r="G51">
-        <v>24</v>
-      </c>
-      <c r="H51" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="356" x14ac:dyDescent="0.2">
-      <c r="A52" s="3">
-        <v>39306</v>
-      </c>
-      <c r="B52" t="s">
-        <v>194</v>
-      </c>
-      <c r="C52" t="s">
-        <v>369</v>
       </c>
       <c r="D52" t="s">
         <v>189</v>
       </c>
       <c r="E52" s="8" t="s">
+        <v>582</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>583</v>
+      </c>
+      <c r="G52">
+        <v>24</v>
+      </c>
+      <c r="H52" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="356" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>39306</v>
+      </c>
+      <c r="B53" t="s">
+        <v>194</v>
+      </c>
+      <c r="C53" t="s">
+        <v>369</v>
+      </c>
+      <c r="D53" t="s">
+        <v>189</v>
+      </c>
+      <c r="E53" s="8" t="s">
         <v>586</v>
       </c>
-      <c r="F52" s="8" t="s">
+      <c r="F53" s="8" t="s">
         <v>587</v>
       </c>
-      <c r="G52">
+      <c r="G53">
         <v>23</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H53" t="s">
         <v>585</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" ht="289" x14ac:dyDescent="0.2">
-      <c r="A53" s="3">
-        <v>39296</v>
-      </c>
-      <c r="B53" t="s">
-        <v>198</v>
-      </c>
-      <c r="C53" t="s">
-        <v>368</v>
-      </c>
-      <c r="D53" t="s">
-        <v>346</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>589</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>590</v>
-      </c>
-      <c r="G53">
-        <v>22</v>
-      </c>
-      <c r="H53" t="s">
-        <v>588</v>
-      </c>
-      <c r="I53" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="289" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
+        <v>39296</v>
+      </c>
+      <c r="B54" t="s">
+        <v>198</v>
+      </c>
+      <c r="C54" t="s">
+        <v>368</v>
+      </c>
+      <c r="D54" t="s">
+        <v>346</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>589</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="G54">
+        <v>22</v>
+      </c>
+      <c r="H54" t="s">
+        <v>588</v>
+      </c>
+      <c r="I54" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="289" x14ac:dyDescent="0.2">
+      <c r="A55" s="3">
         <v>39288</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>201</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>370</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D55" t="s">
         <v>169</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="E55" s="10" t="s">
         <v>592</v>
       </c>
-      <c r="F54" s="8" t="s">
+      <c r="F55" s="8" t="s">
         <v>594</v>
       </c>
-      <c r="G54">
+      <c r="G55">
         <v>21</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H55" t="s">
         <v>593</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I55" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="238" x14ac:dyDescent="0.2">
-      <c r="A55" s="3">
+    <row r="56" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+      <c r="A56" s="3">
         <v>39088</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>209</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>371</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D56" t="s">
         <v>347</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E56" s="8" t="s">
         <v>596</v>
       </c>
-      <c r="F55" s="8" t="s">
+      <c r="F56" s="8" t="s">
         <v>595</v>
       </c>
-      <c r="G55">
+      <c r="G56">
         <v>20</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H56" t="s">
         <v>597</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I56" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="323" x14ac:dyDescent="0.2">
-      <c r="A56" s="3">
-        <v>38926</v>
-      </c>
-      <c r="B56" t="s">
-        <v>213</v>
-      </c>
-      <c r="C56" t="s">
-        <v>372</v>
-      </c>
-      <c r="D56" t="s">
-        <v>348</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>602</v>
-      </c>
-      <c r="F56" s="8" t="s">
-        <v>603</v>
-      </c>
-      <c r="G56">
-        <v>19</v>
-      </c>
-      <c r="H56" t="s">
-        <v>601</v>
-      </c>
-      <c r="I56" s="7" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="323" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>38926</v>
       </c>
       <c r="B57" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C57" t="s">
         <v>372</v>
       </c>
       <c r="D57" t="s">
+        <v>348</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="G57">
+        <v>19</v>
+      </c>
+      <c r="H57" t="s">
+        <v>601</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+      <c r="A58" s="3">
+        <v>38926</v>
+      </c>
+      <c r="B58" t="s">
+        <v>217</v>
+      </c>
+      <c r="C58" t="s">
+        <v>372</v>
+      </c>
+      <c r="D58" t="s">
         <v>216</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="E58" s="10" t="s">
         <v>606</v>
       </c>
-      <c r="F57" s="8" t="s">
+      <c r="F58" s="8" t="s">
         <v>605</v>
       </c>
-      <c r="G57">
+      <c r="G58">
         <v>18</v>
       </c>
-      <c r="H57" t="s">
+      <c r="H58" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="238" x14ac:dyDescent="0.2">
-      <c r="A58" s="3">
+    <row r="59" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+      <c r="A59" s="3">
         <v>38916</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>219</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>373</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>349</v>
       </c>
-      <c r="E58" s="8" t="s">
+      <c r="E59" s="8" t="s">
         <v>609</v>
       </c>
-      <c r="F58" s="8" t="s">
+      <c r="F59" s="8" t="s">
         <v>610</v>
       </c>
-      <c r="G58">
+      <c r="G59">
         <v>17</v>
       </c>
-      <c r="H58" t="s">
+      <c r="H59" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="323" x14ac:dyDescent="0.2">
-      <c r="A59" s="3">
+    <row r="60" spans="1:9" ht="323" x14ac:dyDescent="0.2">
+      <c r="A60" s="3">
         <v>38860</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>225</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>374</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D60" t="s">
         <v>350</v>
       </c>
-      <c r="E59" s="8" t="s">
+      <c r="E60" s="8" t="s">
         <v>611</v>
       </c>
-      <c r="F59" s="8" t="s">
+      <c r="F60" s="8" t="s">
         <v>612</v>
       </c>
-      <c r="G59">
+      <c r="G60">
         <v>16</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H60" t="s">
         <v>613</v>
       </c>
-      <c r="I59" s="7" t="s">
+      <c r="I60" s="7" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="221" x14ac:dyDescent="0.2">
-      <c r="A60" s="3">
+    <row r="61" spans="1:9" ht="221" x14ac:dyDescent="0.2">
+      <c r="A61" s="3">
         <v>38571</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>229</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>375</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D61" t="s">
         <v>228</v>
       </c>
-      <c r="E60" s="8" t="s">
+      <c r="E61" s="8" t="s">
         <v>616</v>
       </c>
-      <c r="F60" s="8" t="s">
+      <c r="F61" s="8" t="s">
         <v>615</v>
       </c>
-      <c r="G60">
+      <c r="G61">
         <v>15</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H61" t="s">
         <v>617</v>
       </c>
-      <c r="I60" s="7" t="s">
+      <c r="I61" s="7" t="s">
         <v>618</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="238" x14ac:dyDescent="0.2">
-      <c r="A61" s="3">
-        <v>38563</v>
-      </c>
-      <c r="B61" t="s">
-        <v>233</v>
-      </c>
-      <c r="C61" t="s">
-        <v>376</v>
-      </c>
-      <c r="D61" t="s">
-        <v>351</v>
-      </c>
-      <c r="E61" s="8" t="s">
-        <v>620</v>
-      </c>
-      <c r="F61" s="8" t="s">
-        <v>621</v>
-      </c>
-      <c r="G61">
-        <v>14</v>
-      </c>
-      <c r="H61" t="s">
-        <v>619</v>
-      </c>
-      <c r="I61" s="7" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="238" x14ac:dyDescent="0.2">
@@ -7440,380 +7475,409 @@
         <v>38563</v>
       </c>
       <c r="B62" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C62" t="s">
         <v>376</v>
       </c>
       <c r="D62" t="s">
+        <v>351</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>620</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>621</v>
+      </c>
+      <c r="G62">
+        <v>14</v>
+      </c>
+      <c r="H62" t="s">
+        <v>619</v>
+      </c>
+      <c r="I62" s="7" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+      <c r="A63" s="3">
+        <v>38563</v>
+      </c>
+      <c r="B63" t="s">
+        <v>237</v>
+      </c>
+      <c r="C63" t="s">
+        <v>376</v>
+      </c>
+      <c r="D63" t="s">
         <v>352</v>
       </c>
-      <c r="E62" s="10" t="s">
+      <c r="E63" s="10" t="s">
         <v>624</v>
       </c>
-      <c r="F62" s="8" t="s">
+      <c r="F63" s="8" t="s">
         <v>625</v>
       </c>
-      <c r="G62">
+      <c r="G63">
         <v>13</v>
       </c>
-      <c r="H62" t="s">
+      <c r="H63" t="s">
         <v>623</v>
       </c>
-      <c r="I62" s="7" t="s">
+      <c r="I63" s="7" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="272" x14ac:dyDescent="0.2">
-      <c r="A63" s="3">
+    <row r="64" spans="1:9" ht="272" x14ac:dyDescent="0.2">
+      <c r="A64" s="3">
         <v>38533</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>239</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>627</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D64" t="s">
         <v>353</v>
       </c>
-      <c r="E63" s="10" t="s">
+      <c r="E64" s="10" t="s">
         <v>629</v>
       </c>
-      <c r="F63" s="8" t="s">
+      <c r="F64" s="8" t="s">
         <v>630</v>
       </c>
-      <c r="G63">
+      <c r="G64">
         <v>12</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H64" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A64" s="3">
+    <row r="65" spans="1:11" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A65" s="3">
         <v>38503</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>633</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>634</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D65" t="s">
         <v>292</v>
       </c>
-      <c r="E64" s="8" t="s">
+      <c r="E65" s="8" t="s">
         <v>635</v>
       </c>
-      <c r="F64" s="8" t="s">
+      <c r="F65" s="8" t="s">
         <v>636</v>
       </c>
-      <c r="G64">
+      <c r="G65">
         <v>11</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H65" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="306" x14ac:dyDescent="0.2">
-      <c r="A65" s="3">
+    <row r="66" spans="1:11" ht="306" x14ac:dyDescent="0.2">
+      <c r="A66" s="3">
         <v>38250</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>246</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>378</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D66" t="s">
         <v>354</v>
       </c>
-      <c r="E65" s="8" t="s">
+      <c r="E66" s="8" t="s">
         <v>638</v>
       </c>
-      <c r="F65" s="8" t="s">
+      <c r="F66" s="8" t="s">
         <v>639</v>
       </c>
-      <c r="G65">
+      <c r="G66">
         <v>10</v>
       </c>
-      <c r="H65" t="s">
+      <c r="H66" t="s">
         <v>640</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="170" x14ac:dyDescent="0.2">
-      <c r="A66" s="3">
-        <v>38222</v>
-      </c>
-      <c r="B66" t="s">
-        <v>250</v>
-      </c>
-      <c r="C66" t="s">
-        <v>379</v>
-      </c>
-      <c r="D66" t="s">
-        <v>352</v>
-      </c>
-      <c r="E66" s="8" t="s">
-        <v>645</v>
-      </c>
-      <c r="F66" s="8" t="s">
-        <v>646</v>
-      </c>
-      <c r="G66">
-        <v>9</v>
-      </c>
-      <c r="H66" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="67" spans="1:11" ht="170" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
+        <v>38222</v>
+      </c>
+      <c r="B67" t="s">
+        <v>250</v>
+      </c>
+      <c r="C67" t="s">
+        <v>379</v>
+      </c>
+      <c r="D67" t="s">
+        <v>352</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="G67">
+        <v>9</v>
+      </c>
+      <c r="H67" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="170" x14ac:dyDescent="0.2">
+      <c r="A68" s="3">
         <v>38114</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>255</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>380</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D68" t="s">
         <v>355</v>
       </c>
-      <c r="E67" s="8" t="s">
+      <c r="E68" s="8" t="s">
         <v>642</v>
       </c>
-      <c r="F67" s="8" t="s">
+      <c r="F68" s="8" t="s">
         <v>641</v>
       </c>
-      <c r="G67">
+      <c r="G68">
         <v>8</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H68" t="s">
         <v>651</v>
       </c>
-      <c r="I67" t="s">
+      <c r="I68" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="238" x14ac:dyDescent="0.2">
-      <c r="A68" s="3">
+    <row r="69" spans="1:11" ht="238" x14ac:dyDescent="0.2">
+      <c r="A69" s="3">
         <v>38113</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>258</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" t="s">
         <v>377</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D69" t="s">
         <v>228</v>
       </c>
-      <c r="E68" s="8" t="s">
+      <c r="E69" s="8" t="s">
         <v>644</v>
       </c>
-      <c r="F68" s="8" t="s">
+      <c r="F69" s="8" t="s">
         <v>643</v>
       </c>
-      <c r="G68">
+      <c r="G69">
         <v>7</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H69" t="s">
         <v>650</v>
       </c>
-      <c r="K68" s="7" t="s">
+      <c r="K69" s="7" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="340" x14ac:dyDescent="0.2">
-      <c r="A69" s="3">
+    <row r="70" spans="1:11" ht="340" x14ac:dyDescent="0.2">
+      <c r="A70" s="3">
         <v>37990</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>260</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
         <v>381</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D70" t="s">
         <v>351</v>
       </c>
-      <c r="E69" s="8" t="s">
+      <c r="E70" s="8" t="s">
         <v>647</v>
       </c>
-      <c r="F69" s="8" t="s">
+      <c r="F70" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="G69">
+      <c r="G70">
         <v>6</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H70" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="372" x14ac:dyDescent="0.2">
-      <c r="A70" s="3">
+    <row r="71" spans="1:11" ht="372" x14ac:dyDescent="0.2">
+      <c r="A71" s="3">
         <v>37579</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>264</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" t="s">
         <v>382</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D71" t="s">
         <v>356</v>
       </c>
-      <c r="E70" s="8" t="s">
+      <c r="E71" s="8" t="s">
         <v>656</v>
       </c>
-      <c r="F70" s="8" t="s">
+      <c r="F71" s="8" t="s">
         <v>657</v>
       </c>
-      <c r="G70">
+      <c r="G71">
         <v>5</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H71" t="s">
         <v>658</v>
       </c>
-      <c r="K70" t="s">
+      <c r="K71" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="272" x14ac:dyDescent="0.2">
-      <c r="A71" s="3">
+    <row r="72" spans="1:11" ht="272" x14ac:dyDescent="0.2">
+      <c r="A72" s="3">
         <v>37494</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>268</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C72" t="s">
         <v>383</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D72" t="s">
         <v>228</v>
       </c>
-      <c r="E71" s="8" t="s">
+      <c r="E72" s="8" t="s">
         <v>653</v>
       </c>
-      <c r="F71" s="8" t="s">
+      <c r="F72" s="8" t="s">
         <v>654</v>
       </c>
-      <c r="G71">
+      <c r="G72">
         <v>4</v>
       </c>
-      <c r="H71" s="16" t="s">
+      <c r="H72" s="16" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="356" x14ac:dyDescent="0.2">
-      <c r="A72" s="3">
+    <row r="73" spans="1:11" ht="356" x14ac:dyDescent="0.2">
+      <c r="A73" s="3">
         <v>37208</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>272</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C73" t="s">
         <v>384</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D73" t="s">
         <v>357</v>
       </c>
-      <c r="E72" s="8" t="s">
+      <c r="E73" s="8" t="s">
         <v>664</v>
       </c>
-      <c r="F72" s="8" t="s">
+      <c r="F73" s="8" t="s">
         <v>665</v>
       </c>
-      <c r="G72">
+      <c r="G73">
         <v>3</v>
       </c>
-      <c r="H72" t="s">
+      <c r="H73" t="s">
         <v>666</v>
       </c>
-      <c r="K72" t="s">
+      <c r="K73" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="272" x14ac:dyDescent="0.2">
-      <c r="A73" s="3">
+    <row r="74" spans="1:11" ht="272" x14ac:dyDescent="0.2">
+      <c r="A74" s="3">
         <v>37107</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B74" t="s">
         <v>275</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C74" t="s">
         <v>385</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D74" t="s">
         <v>228</v>
       </c>
-      <c r="E73" s="8" t="s">
+      <c r="E74" s="8" t="s">
         <v>659</v>
       </c>
-      <c r="F73" s="8" t="s">
+      <c r="F74" s="8" t="s">
         <v>661</v>
       </c>
-      <c r="G73">
+      <c r="G74">
         <v>2</v>
       </c>
-      <c r="H73" t="s">
+      <c r="H74" t="s">
         <v>660</v>
       </c>
-      <c r="K73" s="7" t="s">
+      <c r="K74" s="7" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="340" x14ac:dyDescent="0.2">
-      <c r="A74" s="3">
+    <row r="75" spans="1:11" ht="340" x14ac:dyDescent="0.2">
+      <c r="A75" s="3">
         <v>35638</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>278</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" t="s">
         <v>386</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D75" t="s">
         <v>277</v>
       </c>
-      <c r="E74" s="8" t="s">
+      <c r="E75" s="8" t="s">
         <v>670</v>
       </c>
-      <c r="F74" s="8" t="s">
+      <c r="F75" s="8" t="s">
         <v>668</v>
       </c>
-      <c r="G74">
+      <c r="G75">
         <v>1</v>
       </c>
-      <c r="H74" t="s">
+      <c r="H75" t="s">
         <v>669</v>
       </c>
-      <c r="I74" t="s">
+      <c r="I75" t="s">
         <v>671</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H12" r:id="rId1" display="http://www.aclweb.org/anthology/P17-1167" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="K12" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="K16" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="I35" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="I36" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="I40" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="I41" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="I44" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="I48" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="I45" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="I46" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="I56" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="I59" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="I60" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="I61" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="I62" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="K73" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="K68" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="H13" r:id="rId1" display="http://www.aclweb.org/anthology/P17-1167" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="K13" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="K17" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="I36" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="I37" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="I41" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="I42" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="I45" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="I49" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="I46" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="I47" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="I57" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="I60" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="I61" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="I62" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="I63" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="K74" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="K69" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
update emnlp papers and the code
</commit_message>
<xml_diff>
--- a/markdown_generator/publications.xlsx
+++ b/markdown_generator/publications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottyih/GitHub/scottyih.github.io/markdown_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F974CBDE-68EE-0341-A804-2E5F1A4F2ED3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135C09CB-AED3-C24E-ADF0-568659EDFD97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="460" yWindow="660" windowWidth="30000" windowHeight="18220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="710">
   <si>
     <t>Po-Sen Huang, Chenglong Wang, Rishabh Singh, Wen-tau Yih and Xiaodong He</t>
   </si>
@@ -3549,7 +3549,41 @@
 org/propara</t>
   </si>
   <si>
-    <t>"@InProceedings{mishra-EtAl:2019,
+    <t>MishraTandon-emnlp19.pdf</t>
+  </si>
+  <si>
+    <t>Model-based Interactive Semantic Parsing: A Unified Framework and A Text-to-SQL Case Study</t>
+  </si>
+  <si>
+    <t>Ziyu Yao, Yu Su, Huan Sun, Wen-tau Yih</t>
+  </si>
+  <si>
+    <t>As a promising paradigm, interactive semantic
+parsing has shown to improve both semantic
+parsing accuracy and user confidence in the results.
+In this paper, we propose a new, unified
+formulation of the interactive semantic parsing
+problem, where the goal is to design a modelbased
+intelligent agent. The agent maintains
+its own state as the current predicted semantic
+parse, decides whether and where human intervention
+is needed, and generates a clarification
+question in natural language. A key part of the
+agent is a world model: it takes a percept (either
+an initial question or subsequent feedback
+from the user) and transitions to a new state.
+We then propose a simple yet remarkably effective
+instantiation of our framework, demonstrated
+on two text-to-SQL datasets (WikiSQL
+and Spider) with different state-of-the-art base
+semantic parsers. Compared to an existing interactive
+semantic parsing approach that treats
+the base parser as a black box, our approach
+solicits less user feedback but yields higher
+run-time accuracy</t>
+  </si>
+  <si>
+    <t>@InProceedings{mishra-EtAl:2019,
   author    = {Bhavana Dalvi Mishra and Niket Tandon and Antoine Bosselut and Wen-tau Yih and Peter Clark},
   title     = {Everything Happens for a Reason: Discovering the Purpose of Actions in Procedural Text},
   booktitle = {Proceedings of the 2019 Conference on Empirical Methods in Natural Language Processing},
@@ -3557,10 +3591,24 @@
   year      = {2019},
   address   = {Hong Kong, China},
   publisher = {Association for Computational Linguistics},
-}"</t>
-  </si>
-  <si>
-    <t>MishraTandon-emnlp19.pdf</t>
+}</t>
+  </si>
+  <si>
+    <t>@InProceedings{mishra-EtAl:2019,
+  author    = {Ziyu Yao and Yu Su and Huan Sun and Wen-tau Yih},
+  title     = {Model-based Interactive Semantic Parsing: A Unified Framework and A Text-to-SQL Case Study},
+  booktitle = {Proceedings of the 2019 Conference on Empirical Methods in Natural Language Processing},
+  month     = {November},
+  year      = {2019},
+  address   = {Hong Kong, China},
+  publisher = {Association for Computational Linguistics},
+}</t>
+  </si>
+  <si>
+    <t>https://github.com/sunlab-osu/MISP</t>
+  </si>
+  <si>
+    <t>YaoSuSunYih-emnlp19-misp.pdf</t>
   </si>
 </sst>
 </file>
@@ -4083,7 +4131,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -4115,6 +4163,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="34" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="34" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -5717,11 +5766,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M76"/>
+  <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5782,1790 +5831,1790 @@
         <v>389</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" ht="356" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="5" customFormat="1" ht="388" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>43772</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>697</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>704</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>705</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>707</v>
+      </c>
+      <c r="G2" s="5">
+        <v>76</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>709</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="5" customFormat="1" ht="356" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>43772</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>700</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>697</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>699</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>701</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F3" s="15" t="s">
+        <v>706</v>
+      </c>
+      <c r="G3" s="5">
+        <v>75</v>
+      </c>
+      <c r="H3" s="14" t="s">
         <v>702</v>
       </c>
-      <c r="G2" s="5">
-        <v>75</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>703</v>
-      </c>
-      <c r="K2" s="18" t="s">
+      <c r="K3" s="18" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" ht="340" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+    <row r="4" spans="1:13" s="5" customFormat="1" ht="340" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
         <v>43619</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="5" t="s">
         <v>692</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>693</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>698</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E4" s="15" t="s">
         <v>695</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F4" s="15" t="s">
         <v>696</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G4" s="5">
         <v>74</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>694</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" ht="289" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+    <row r="5" spans="1:13" s="5" customFormat="1" ht="289" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
         <v>43591</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>686</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>690</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>687</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E5" s="13" t="s">
         <v>688</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F5" s="15" t="s">
         <v>691</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G5" s="5">
         <v>73</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>684</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="5" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+    <row r="6" spans="1:13" s="5" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
         <v>43492</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B6" s="5" t="s">
         <v>677</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>678</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>679</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E6" s="13" t="s">
         <v>689</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F6" s="15" t="s">
         <v>683</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G6" s="5">
         <v>72</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>682</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="5" customFormat="1" ht="306" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
-        <v>43404</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>398</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>393</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>631</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>461</v>
-      </c>
-      <c r="G6">
-        <v>71</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>454</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="5" customFormat="1" ht="372" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="5" customFormat="1" ht="306" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>43404</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>393</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G7">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>681</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" s="5" customFormat="1" ht="404" x14ac:dyDescent="0.2">
+        <v>454</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="5" customFormat="1" ht="372" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>43404</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>673</v>
+        <v>396</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>394</v>
+      <c r="D8" s="5" t="s">
+        <v>395</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>459</v>
+        <v>632</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>676</v>
+        <v>462</v>
       </c>
       <c r="G8">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="5" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
+        <v>456</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>681</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="5" customFormat="1" ht="404" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>43404</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>392</v>
+        <v>673</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>393</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>459</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>676</v>
+      </c>
+      <c r="G9">
+        <v>69</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="5" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>43404</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>674</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E10" s="13" t="s">
         <v>460</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F10" s="15" t="s">
         <v>675</v>
       </c>
-      <c r="G9">
+      <c r="G10">
         <v>68</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H10" s="14" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="259" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
-        <v>43253</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>294</v>
-      </c>
-      <c r="D10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>414</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>415</v>
-      </c>
-      <c r="G10">
-        <v>67</v>
-      </c>
-      <c r="H10" t="s">
-        <v>413</v>
-      </c>
-      <c r="L10" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="291" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="259" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>43253</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>294</v>
       </c>
       <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="G11">
+        <v>67</v>
+      </c>
+      <c r="H11" t="s">
+        <v>413</v>
+      </c>
+      <c r="L11" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="291" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>43253</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>294</v>
+      </c>
+      <c r="D12" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E12" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="G11">
+      <c r="G12">
         <v>66</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H12" t="s">
         <v>416</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K12" t="s">
         <v>417</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L12" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="272" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+    <row r="13" spans="1:13" ht="272" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
         <v>43133</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>295</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E13" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>423</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>65</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H13" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="340" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+    <row r="14" spans="1:13" ht="340" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
         <v>42985</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>296</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>425</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>64</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H14" t="s">
         <v>426</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J14" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="345" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
-        <v>42946</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
-        <v>297</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>403</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="G14">
-        <v>63</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>400</v>
-      </c>
-      <c r="I14" t="s">
-        <v>406</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>404</v>
-      </c>
-      <c r="L14" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="404" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="345" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>42946</v>
       </c>
       <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>297</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="G15">
+        <v>63</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="I15" t="s">
+        <v>406</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="L15" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="404" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>42946</v>
+      </c>
+      <c r="B16" t="s">
         <v>22</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>298</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E16" s="8" t="s">
         <v>428</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F16" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="G15">
+      <c r="G16">
         <v>62</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="H16" s="11" t="s">
         <v>427</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J16" t="s">
         <v>452</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K16" t="s">
         <v>407</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L16" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="306" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+    <row r="17" spans="1:13" ht="306" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
         <v>42675</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>299</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E17" s="8" t="s">
         <v>432</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F17" s="8" t="s">
         <v>431</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>61</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H17" t="s">
         <v>430</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J17" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="372" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
-        <v>42589</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>300</v>
-      </c>
-      <c r="D17" t="s">
-        <v>358</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>439</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>438</v>
-      </c>
-      <c r="G17">
-        <v>60</v>
-      </c>
-      <c r="H17" t="s">
-        <v>437</v>
-      </c>
-      <c r="J17" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="272" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="372" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>42589</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
         <v>300</v>
       </c>
       <c r="D18" t="s">
+        <v>358</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="G18">
+        <v>60</v>
+      </c>
+      <c r="H18" t="s">
+        <v>437</v>
+      </c>
+      <c r="J18" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="272" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>42589</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>300</v>
+      </c>
+      <c r="D19" t="s">
         <v>319</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E19" s="8" t="s">
         <v>442</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F19" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="G18">
+      <c r="G19">
         <v>59</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H19" t="s">
         <v>440</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I19" t="s">
         <v>444</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="K19" s="7" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="356" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+    <row r="20" spans="1:13" ht="356" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
         <v>42492</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>38</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>301</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>320</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E20" s="8" t="s">
         <v>446</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F20" s="8" t="s">
         <v>447</v>
       </c>
-      <c r="G19">
+      <c r="G20">
         <v>58</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H20" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+    <row r="21" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
         <v>42471</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>305</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>321</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>449</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F21" s="8" t="s">
         <v>450</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <v>57</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H21" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="388" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+    <row r="22" spans="1:13" ht="388" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
         <v>42264</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>47</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>303</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>322</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E22" s="10" t="s">
         <v>464</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F22" s="8" t="s">
         <v>463</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <v>56</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H22" t="s">
         <v>465</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I22" t="s">
         <v>468</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K22" t="s">
         <v>466</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L22" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="323" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
+    <row r="23" spans="1:13" ht="323" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
         <v>42213</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>50</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>304</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>323</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E23" s="10" t="s">
         <v>472</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F23" s="8" t="s">
         <v>471</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <v>55</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H23" t="s">
         <v>473</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I23" t="s">
         <v>469</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J23" t="s">
         <v>451</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L23" t="s">
         <v>470</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M23" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="388" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
+    <row r="24" spans="1:13" ht="388" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
         <v>42125</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>57</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>306</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>324</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E24" s="10" t="s">
         <v>475</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F24" s="8" t="s">
         <v>476</v>
       </c>
-      <c r="G23">
+      <c r="G24">
         <v>54</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H24" t="s">
         <v>474</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I24" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="404" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
-        <v>42144</v>
-      </c>
-      <c r="B24" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" t="s">
-        <v>302</v>
-      </c>
-      <c r="D24" t="s">
-        <v>325</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>480</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>482</v>
-      </c>
-      <c r="G24">
-        <v>53</v>
-      </c>
-      <c r="H24" t="s">
-        <v>481</v>
-      </c>
-      <c r="I24" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="404" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>42144</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
         <v>302</v>
       </c>
       <c r="D25" t="s">
+        <v>325</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>480</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="G25">
+        <v>53</v>
+      </c>
+      <c r="H25" t="s">
+        <v>481</v>
+      </c>
+      <c r="I25" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>42144</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="s">
+        <v>302</v>
+      </c>
+      <c r="D26" t="s">
         <v>326</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E26" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F26" s="8" t="s">
         <v>483</v>
       </c>
-      <c r="G25">
+      <c r="G26">
         <v>52</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H26" t="s">
         <v>485</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I26" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="289" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+    <row r="27" spans="1:13" ht="289" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
         <v>42244</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>66</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>307</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>327</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E27" s="10" t="s">
         <v>488</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F27" s="8" t="s">
         <v>487</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <v>51</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H27" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+    <row r="28" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
         <v>41983</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>73</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>308</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>328</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E28" s="10" t="s">
         <v>490</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F28" s="8" t="s">
         <v>491</v>
       </c>
-      <c r="G27">
+      <c r="G28">
         <v>50</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H28" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="404" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+    <row r="29" spans="1:13" ht="404" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
         <v>41937</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>81</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>309</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>329</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E29" s="10" t="s">
         <v>493</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F29" s="8" t="s">
         <v>494</v>
       </c>
-      <c r="G28">
+      <c r="G29">
         <v>49</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H29" t="s">
         <v>492</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I29" t="s">
         <v>495</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J29" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="340" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
-        <v>41813</v>
-      </c>
-      <c r="B29" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" t="s">
-        <v>388</v>
-      </c>
-      <c r="D29" t="s">
-        <v>330</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>497</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>498</v>
-      </c>
-      <c r="G29">
-        <v>48</v>
-      </c>
-      <c r="H29" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="306" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="340" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>41813</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
         <v>388</v>
       </c>
       <c r="D30" t="s">
+        <v>330</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>498</v>
+      </c>
+      <c r="G30">
+        <v>48</v>
+      </c>
+      <c r="H30" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="306" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>41813</v>
+      </c>
+      <c r="B31" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" t="s">
+        <v>388</v>
+      </c>
+      <c r="D31" t="s">
         <v>331</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E31" s="8" t="s">
         <v>500</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F31" s="8" t="s">
         <v>501</v>
       </c>
-      <c r="G30">
+      <c r="G31">
         <v>47</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H31" t="s">
         <v>499</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I31" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="221" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
-        <v>41565</v>
-      </c>
-      <c r="B31" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" t="s">
-        <v>399</v>
-      </c>
-      <c r="D31" t="s">
-        <v>332</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>504</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>505</v>
-      </c>
-      <c r="G31">
-        <v>46</v>
-      </c>
-      <c r="H31" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="323" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>41565</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C32" t="s">
         <v>399</v>
       </c>
       <c r="D32" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="G32">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H32" t="s">
-        <v>509</v>
-      </c>
-      <c r="I32" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="323" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
+        <v>41565</v>
+      </c>
+      <c r="B33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" t="s">
+        <v>399</v>
+      </c>
+      <c r="D33" t="s">
+        <v>333</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>507</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="G33">
+        <v>45</v>
+      </c>
+      <c r="H33" t="s">
+        <v>509</v>
+      </c>
+      <c r="I33" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="323" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
         <v>41490</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>101</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>503</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>334</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E34" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="F33" s="8" t="s">
+      <c r="F34" s="8" t="s">
         <v>512</v>
       </c>
-      <c r="G33">
+      <c r="G34">
         <v>44</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H34" t="s">
         <v>513</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I34" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
-        <v>41421</v>
-      </c>
-      <c r="B34" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" t="s">
-        <v>310</v>
-      </c>
-      <c r="D34" t="s">
-        <v>335</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>518</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>517</v>
-      </c>
-      <c r="G34">
-        <v>43</v>
-      </c>
-      <c r="H34" t="s">
-        <v>516</v>
-      </c>
-      <c r="K34" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="238" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>41421</v>
       </c>
       <c r="B35" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C35" t="s">
         <v>310</v>
       </c>
       <c r="D35" t="s">
+        <v>335</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>518</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>517</v>
+      </c>
+      <c r="G35">
+        <v>43</v>
+      </c>
+      <c r="H35" t="s">
+        <v>516</v>
+      </c>
+      <c r="K35" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="238" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
+        <v>41421</v>
+      </c>
+      <c r="B36" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" t="s">
+        <v>310</v>
+      </c>
+      <c r="D36" t="s">
         <v>336</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E36" s="10" t="s">
         <v>520</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F36" s="8" t="s">
         <v>521</v>
       </c>
-      <c r="G35">
+      <c r="G36">
         <v>42</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H36" t="s">
         <v>519</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I36" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="356" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
+    <row r="37" spans="1:13" ht="356" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
         <v>41565</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>111</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>298</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>110</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E37" s="10" t="s">
         <v>524</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F37" s="8" t="s">
         <v>526</v>
       </c>
-      <c r="G36">
+      <c r="G37">
         <v>41</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H37" t="s">
         <v>523</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I37" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="372" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
+    <row r="38" spans="1:13" ht="372" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
         <v>41102</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>116</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>311</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>337</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E38" s="10" t="s">
         <v>528</v>
       </c>
-      <c r="F37" s="8" t="s">
+      <c r="F38" s="8" t="s">
         <v>527</v>
       </c>
-      <c r="G37">
+      <c r="G38">
         <v>40</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H38" t="s">
         <v>529</v>
       </c>
-      <c r="I37" s="7" t="s">
+      <c r="I38" s="7" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="221" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
-        <v>41062</v>
-      </c>
-      <c r="B38" t="s">
-        <v>120</v>
-      </c>
-      <c r="C38" t="s">
-        <v>312</v>
-      </c>
-      <c r="D38" t="s">
-        <v>119</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>532</v>
-      </c>
-      <c r="F38" s="8" t="s">
-        <v>533</v>
-      </c>
-      <c r="G38">
-        <v>39</v>
-      </c>
-      <c r="H38" t="s">
-        <v>531</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="255" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>41062</v>
       </c>
       <c r="B39" t="s">
-        <v>313</v>
+        <v>120</v>
       </c>
       <c r="C39" t="s">
         <v>312</v>
       </c>
       <c r="D39" t="s">
+        <v>119</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="G39">
+        <v>39</v>
+      </c>
+      <c r="H39" t="s">
+        <v>531</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="255" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>41062</v>
+      </c>
+      <c r="B40" t="s">
+        <v>313</v>
+      </c>
+      <c r="C40" t="s">
+        <v>312</v>
+      </c>
+      <c r="D40" t="s">
         <v>338</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E40" s="10" t="s">
         <v>535</v>
       </c>
-      <c r="F39" s="8" t="s">
+      <c r="F40" s="8" t="s">
         <v>536</v>
       </c>
-      <c r="G39">
+      <c r="G40">
         <v>38</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H40" t="s">
         <v>537</v>
       </c>
-      <c r="L39" t="s">
+      <c r="L40" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
+    <row r="41" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
         <v>40748</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>129</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>314</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>339</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E41" s="8" t="s">
         <v>540</v>
       </c>
-      <c r="F40" s="8" t="s">
+      <c r="F41" s="8" t="s">
         <v>539</v>
       </c>
-      <c r="G40">
+      <c r="G41">
         <v>37</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H41" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="306" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
+    <row r="42" spans="1:13" ht="306" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
         <v>40740</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>134</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>315</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>133</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E42" s="10" t="s">
         <v>543</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="F42" s="8" t="s">
         <v>542</v>
       </c>
-      <c r="G41">
+      <c r="G42">
         <v>36</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H42" t="s">
         <v>544</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I42" t="s">
         <v>549</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J42" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="289" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
+    <row r="43" spans="1:13" ht="289" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
         <v>40707</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>138</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>316</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>340</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E43" s="10" t="s">
         <v>547</v>
       </c>
-      <c r="F42" s="8" t="s">
+      <c r="F43" s="8" t="s">
         <v>545</v>
       </c>
-      <c r="G42">
+      <c r="G43">
         <v>35</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H43" t="s">
         <v>546</v>
       </c>
-      <c r="I42" s="7" t="s">
+      <c r="I43" s="7" t="s">
         <v>548</v>
       </c>
-      <c r="M42" t="s">
+      <c r="M43" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="323" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
+    <row r="44" spans="1:13" ht="323" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
         <v>40522</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>142</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>317</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>141</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E44" s="10" t="s">
         <v>551</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="F44" s="8" t="s">
         <v>550</v>
       </c>
-      <c r="G43">
+      <c r="G44">
         <v>34</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H44" t="s">
         <v>552</v>
       </c>
-      <c r="I43" s="7" t="s">
+      <c r="I44" s="7" t="s">
         <v>553</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
-        <v>40460</v>
-      </c>
-      <c r="B44" t="s">
-        <v>150</v>
-      </c>
-      <c r="C44" t="s">
-        <v>318</v>
-      </c>
-      <c r="D44" t="s">
-        <v>341</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>555</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>554</v>
-      </c>
-      <c r="G44">
-        <v>33</v>
-      </c>
-      <c r="H44" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
+        <v>40460</v>
+      </c>
+      <c r="B45" t="s">
+        <v>150</v>
+      </c>
+      <c r="C45" t="s">
+        <v>318</v>
+      </c>
+      <c r="D45" t="s">
+        <v>341</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>555</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>554</v>
+      </c>
+      <c r="G45">
+        <v>33</v>
+      </c>
+      <c r="H45" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
         <v>40378</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>154</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>387</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>342</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E46" s="10" t="s">
         <v>558</v>
       </c>
-      <c r="F45" s="8" t="s">
+      <c r="F46" s="8" t="s">
         <v>557</v>
       </c>
-      <c r="G45">
+      <c r="G46">
         <v>32</v>
       </c>
-      <c r="H45" t="s">
+      <c r="H46" t="s">
         <v>559</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I46" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="388" x14ac:dyDescent="0.2">
-      <c r="A46" s="3">
+    <row r="47" spans="1:13" ht="388" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
         <v>40032</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>359</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>360</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>292</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E47" s="10" t="s">
         <v>562</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="F47" s="8" t="s">
         <v>561</v>
       </c>
-      <c r="G46">
+      <c r="G47">
         <v>31</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H47" t="s">
         <v>563</v>
       </c>
-      <c r="I46" s="7" t="s">
+      <c r="I47" s="7" t="s">
         <v>564</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A47" s="3">
-        <v>40011</v>
-      </c>
-      <c r="B47" t="s">
-        <v>161</v>
-      </c>
-      <c r="C47" t="s">
-        <v>361</v>
-      </c>
-      <c r="D47" t="s">
-        <v>160</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>575</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="G47">
-        <v>30</v>
-      </c>
-      <c r="H47" t="s">
-        <v>574</v>
-      </c>
-      <c r="I47" s="7" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
-        <v>39684</v>
+        <v>40011</v>
       </c>
       <c r="B48" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C48" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D48" t="s">
-        <v>343</v>
+        <v>160</v>
       </c>
       <c r="E48" s="10" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="G48">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H48" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="306" x14ac:dyDescent="0.2">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>39684</v>
       </c>
       <c r="B49" t="s">
+        <v>166</v>
+      </c>
+      <c r="C49" t="s">
+        <v>362</v>
+      </c>
+      <c r="D49" t="s">
+        <v>343</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>579</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="G49">
+        <v>29</v>
+      </c>
+      <c r="H49" t="s">
+        <v>578</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="306" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
+        <v>39684</v>
+      </c>
+      <c r="B50" t="s">
         <v>170</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>363</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>169</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E50" s="8" t="s">
         <v>434</v>
       </c>
-      <c r="F49" s="8" t="s">
+      <c r="F50" s="8" t="s">
         <v>435</v>
       </c>
-      <c r="G49">
+      <c r="G50">
         <v>28</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H50" t="s">
         <v>433</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I50" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="238" x14ac:dyDescent="0.2">
-      <c r="A50" s="3">
+    <row r="51" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
         <v>39681</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>174</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>364</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>344</v>
       </c>
-      <c r="E50" s="10" t="s">
+      <c r="E51" s="10" t="s">
         <v>566</v>
       </c>
-      <c r="F50" s="8" t="s">
+      <c r="F51" s="8" t="s">
         <v>567</v>
       </c>
-      <c r="G50">
+      <c r="G51">
         <v>27</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H51" t="s">
         <v>565</v>
       </c>
-      <c r="I50" s="7" t="s">
+      <c r="I51" s="7" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="356" x14ac:dyDescent="0.2">
-      <c r="A51" s="3">
+    <row r="52" spans="1:9" ht="356" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
         <v>39173</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>178</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>365</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>345</v>
       </c>
-      <c r="E51" s="8" t="s">
+      <c r="E52" s="8" t="s">
         <v>570</v>
       </c>
-      <c r="F51" s="8" t="s">
+      <c r="F52" s="8" t="s">
         <v>571</v>
       </c>
-      <c r="G51">
+      <c r="G52">
         <v>26</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H52" t="s">
         <v>569</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A52" s="3">
-        <v>39416</v>
-      </c>
-      <c r="B52" t="s">
-        <v>185</v>
-      </c>
-      <c r="C52" t="s">
-        <v>366</v>
-      </c>
-      <c r="D52" t="s">
-        <v>184</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>573</v>
-      </c>
-      <c r="F52" s="8" t="s">
-        <v>591</v>
-      </c>
-      <c r="G52">
-        <v>25</v>
-      </c>
-      <c r="H52" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
+        <v>39416</v>
+      </c>
+      <c r="B53" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53" t="s">
+        <v>366</v>
+      </c>
+      <c r="D53" t="s">
+        <v>184</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>573</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>591</v>
+      </c>
+      <c r="G53">
+        <v>25</v>
+      </c>
+      <c r="H53" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A54" s="3">
         <v>39345</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>190</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>367</v>
-      </c>
-      <c r="D53" t="s">
-        <v>189</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>582</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>583</v>
-      </c>
-      <c r="G53">
-        <v>24</v>
-      </c>
-      <c r="H53" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" ht="356" x14ac:dyDescent="0.2">
-      <c r="A54" s="3">
-        <v>39306</v>
-      </c>
-      <c r="B54" t="s">
-        <v>194</v>
-      </c>
-      <c r="C54" t="s">
-        <v>369</v>
       </c>
       <c r="D54" t="s">
         <v>189</v>
       </c>
       <c r="E54" s="8" t="s">
+        <v>582</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>583</v>
+      </c>
+      <c r="G54">
+        <v>24</v>
+      </c>
+      <c r="H54" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="356" x14ac:dyDescent="0.2">
+      <c r="A55" s="3">
+        <v>39306</v>
+      </c>
+      <c r="B55" t="s">
+        <v>194</v>
+      </c>
+      <c r="C55" t="s">
+        <v>369</v>
+      </c>
+      <c r="D55" t="s">
+        <v>189</v>
+      </c>
+      <c r="E55" s="8" t="s">
         <v>586</v>
       </c>
-      <c r="F54" s="8" t="s">
+      <c r="F55" s="8" t="s">
         <v>587</v>
       </c>
-      <c r="G54">
+      <c r="G55">
         <v>23</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H55" t="s">
         <v>585</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="289" x14ac:dyDescent="0.2">
-      <c r="A55" s="3">
-        <v>39296</v>
-      </c>
-      <c r="B55" t="s">
-        <v>198</v>
-      </c>
-      <c r="C55" t="s">
-        <v>368</v>
-      </c>
-      <c r="D55" t="s">
-        <v>346</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>589</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>590</v>
-      </c>
-      <c r="G55">
-        <v>22</v>
-      </c>
-      <c r="H55" t="s">
-        <v>588</v>
-      </c>
-      <c r="I55" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="289" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
+        <v>39296</v>
+      </c>
+      <c r="B56" t="s">
+        <v>198</v>
+      </c>
+      <c r="C56" t="s">
+        <v>368</v>
+      </c>
+      <c r="D56" t="s">
+        <v>346</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>589</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="G56">
+        <v>22</v>
+      </c>
+      <c r="H56" t="s">
+        <v>588</v>
+      </c>
+      <c r="I56" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="289" x14ac:dyDescent="0.2">
+      <c r="A57" s="3">
         <v>39288</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>201</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>370</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>169</v>
       </c>
-      <c r="E56" s="10" t="s">
+      <c r="E57" s="10" t="s">
         <v>592</v>
       </c>
-      <c r="F56" s="8" t="s">
+      <c r="F57" s="8" t="s">
         <v>594</v>
       </c>
-      <c r="G56">
+      <c r="G57">
         <v>21</v>
       </c>
-      <c r="H56" t="s">
+      <c r="H57" t="s">
         <v>593</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I57" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="238" x14ac:dyDescent="0.2">
-      <c r="A57" s="3">
+    <row r="58" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+      <c r="A58" s="3">
         <v>39088</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>209</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>371</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>347</v>
       </c>
-      <c r="E57" s="8" t="s">
+      <c r="E58" s="8" t="s">
         <v>596</v>
       </c>
-      <c r="F57" s="8" t="s">
+      <c r="F58" s="8" t="s">
         <v>595</v>
       </c>
-      <c r="G57">
+      <c r="G58">
         <v>20</v>
       </c>
-      <c r="H57" t="s">
+      <c r="H58" t="s">
         <v>597</v>
       </c>
-      <c r="I57" t="s">
+      <c r="I58" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="323" x14ac:dyDescent="0.2">
-      <c r="A58" s="3">
-        <v>38926</v>
-      </c>
-      <c r="B58" t="s">
-        <v>213</v>
-      </c>
-      <c r="C58" t="s">
-        <v>372</v>
-      </c>
-      <c r="D58" t="s">
-        <v>348</v>
-      </c>
-      <c r="E58" s="10" t="s">
-        <v>602</v>
-      </c>
-      <c r="F58" s="8" t="s">
-        <v>603</v>
-      </c>
-      <c r="G58">
-        <v>19</v>
-      </c>
-      <c r="H58" t="s">
-        <v>601</v>
-      </c>
-      <c r="I58" s="7" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="323" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>38926</v>
       </c>
       <c r="B59" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C59" t="s">
         <v>372</v>
       </c>
       <c r="D59" t="s">
+        <v>348</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="G59">
+        <v>19</v>
+      </c>
+      <c r="H59" t="s">
+        <v>601</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+      <c r="A60" s="3">
+        <v>38926</v>
+      </c>
+      <c r="B60" t="s">
+        <v>217</v>
+      </c>
+      <c r="C60" t="s">
+        <v>372</v>
+      </c>
+      <c r="D60" t="s">
         <v>216</v>
       </c>
-      <c r="E59" s="10" t="s">
+      <c r="E60" s="10" t="s">
         <v>606</v>
       </c>
-      <c r="F59" s="8" t="s">
+      <c r="F60" s="8" t="s">
         <v>605</v>
       </c>
-      <c r="G59">
+      <c r="G60">
         <v>18</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H60" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="238" x14ac:dyDescent="0.2">
-      <c r="A60" s="3">
+    <row r="61" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+      <c r="A61" s="3">
         <v>38916</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>219</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>373</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D61" t="s">
         <v>349</v>
       </c>
-      <c r="E60" s="8" t="s">
+      <c r="E61" s="8" t="s">
         <v>609</v>
       </c>
-      <c r="F60" s="8" t="s">
+      <c r="F61" s="8" t="s">
         <v>610</v>
       </c>
-      <c r="G60">
+      <c r="G61">
         <v>17</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H61" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="323" x14ac:dyDescent="0.2">
-      <c r="A61" s="3">
+    <row r="62" spans="1:9" ht="323" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
         <v>38860</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>225</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>374</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D62" t="s">
         <v>350</v>
       </c>
-      <c r="E61" s="8" t="s">
+      <c r="E62" s="8" t="s">
         <v>611</v>
       </c>
-      <c r="F61" s="8" t="s">
+      <c r="F62" s="8" t="s">
         <v>612</v>
       </c>
-      <c r="G61">
+      <c r="G62">
         <v>16</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H62" t="s">
         <v>613</v>
       </c>
-      <c r="I61" s="7" t="s">
+      <c r="I62" s="7" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="221" x14ac:dyDescent="0.2">
-      <c r="A62" s="3">
+    <row r="63" spans="1:9" ht="221" x14ac:dyDescent="0.2">
+      <c r="A63" s="3">
         <v>38571</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>229</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>375</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D63" t="s">
         <v>228</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="E63" s="8" t="s">
         <v>616</v>
       </c>
-      <c r="F62" s="8" t="s">
+      <c r="F63" s="8" t="s">
         <v>615</v>
       </c>
-      <c r="G62">
+      <c r="G63">
         <v>15</v>
       </c>
-      <c r="H62" t="s">
+      <c r="H63" t="s">
         <v>617</v>
       </c>
-      <c r="I62" s="7" t="s">
+      <c r="I63" s="7" t="s">
         <v>618</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="238" x14ac:dyDescent="0.2">
-      <c r="A63" s="3">
-        <v>38563</v>
-      </c>
-      <c r="B63" t="s">
-        <v>233</v>
-      </c>
-      <c r="C63" t="s">
-        <v>376</v>
-      </c>
-      <c r="D63" t="s">
-        <v>351</v>
-      </c>
-      <c r="E63" s="8" t="s">
-        <v>620</v>
-      </c>
-      <c r="F63" s="8" t="s">
-        <v>621</v>
-      </c>
-      <c r="G63">
-        <v>14</v>
-      </c>
-      <c r="H63" t="s">
-        <v>619</v>
-      </c>
-      <c r="I63" s="7" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="238" x14ac:dyDescent="0.2">
@@ -7573,381 +7622,411 @@
         <v>38563</v>
       </c>
       <c r="B64" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C64" t="s">
         <v>376</v>
       </c>
       <c r="D64" t="s">
+        <v>351</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>620</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>621</v>
+      </c>
+      <c r="G64">
+        <v>14</v>
+      </c>
+      <c r="H64" t="s">
+        <v>619</v>
+      </c>
+      <c r="I64" s="7" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="238" x14ac:dyDescent="0.2">
+      <c r="A65" s="3">
+        <v>38563</v>
+      </c>
+      <c r="B65" t="s">
+        <v>237</v>
+      </c>
+      <c r="C65" t="s">
+        <v>376</v>
+      </c>
+      <c r="D65" t="s">
         <v>352</v>
       </c>
-      <c r="E64" s="10" t="s">
+      <c r="E65" s="10" t="s">
         <v>624</v>
       </c>
-      <c r="F64" s="8" t="s">
+      <c r="F65" s="8" t="s">
         <v>625</v>
       </c>
-      <c r="G64">
+      <c r="G65">
         <v>13</v>
       </c>
-      <c r="H64" t="s">
+      <c r="H65" t="s">
         <v>623</v>
       </c>
-      <c r="I64" s="7" t="s">
+      <c r="I65" s="7" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="272" x14ac:dyDescent="0.2">
-      <c r="A65" s="3">
+    <row r="66" spans="1:11" ht="272" x14ac:dyDescent="0.2">
+      <c r="A66" s="3">
         <v>38533</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>239</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>627</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D66" t="s">
         <v>353</v>
       </c>
-      <c r="E65" s="10" t="s">
+      <c r="E66" s="10" t="s">
         <v>629</v>
       </c>
-      <c r="F65" s="8" t="s">
+      <c r="F66" s="8" t="s">
         <v>630</v>
       </c>
-      <c r="G65">
+      <c r="G66">
         <v>12</v>
       </c>
-      <c r="H65" t="s">
+      <c r="H66" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A66" s="3">
+    <row r="67" spans="1:11" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A67" s="3">
         <v>38503</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>633</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C67" t="s">
         <v>634</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D67" t="s">
         <v>292</v>
       </c>
-      <c r="E66" s="8" t="s">
+      <c r="E67" s="8" t="s">
         <v>635</v>
       </c>
-      <c r="F66" s="8" t="s">
+      <c r="F67" s="8" t="s">
         <v>636</v>
       </c>
-      <c r="G66">
+      <c r="G67">
         <v>11</v>
       </c>
-      <c r="H66" t="s">
+      <c r="H67" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="306" x14ac:dyDescent="0.2">
-      <c r="A67" s="3">
+    <row r="68" spans="1:11" ht="306" x14ac:dyDescent="0.2">
+      <c r="A68" s="3">
         <v>38250</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>246</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>378</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D68" t="s">
         <v>354</v>
       </c>
-      <c r="E67" s="8" t="s">
+      <c r="E68" s="8" t="s">
         <v>638</v>
       </c>
-      <c r="F67" s="8" t="s">
+      <c r="F68" s="8" t="s">
         <v>639</v>
       </c>
-      <c r="G67">
+      <c r="G68">
         <v>10</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H68" t="s">
         <v>640</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="170" x14ac:dyDescent="0.2">
-      <c r="A68" s="3">
-        <v>38222</v>
-      </c>
-      <c r="B68" t="s">
-        <v>250</v>
-      </c>
-      <c r="C68" t="s">
-        <v>379</v>
-      </c>
-      <c r="D68" t="s">
-        <v>352</v>
-      </c>
-      <c r="E68" s="8" t="s">
-        <v>645</v>
-      </c>
-      <c r="F68" s="8" t="s">
-        <v>646</v>
-      </c>
-      <c r="G68">
-        <v>9</v>
-      </c>
-      <c r="H68" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="69" spans="1:11" ht="170" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
+        <v>38222</v>
+      </c>
+      <c r="B69" t="s">
+        <v>250</v>
+      </c>
+      <c r="C69" t="s">
+        <v>379</v>
+      </c>
+      <c r="D69" t="s">
+        <v>352</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>645</v>
+      </c>
+      <c r="F69" s="8" t="s">
+        <v>646</v>
+      </c>
+      <c r="G69">
+        <v>9</v>
+      </c>
+      <c r="H69" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="170" x14ac:dyDescent="0.2">
+      <c r="A70" s="3">
         <v>38114</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>255</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
         <v>380</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D70" t="s">
         <v>355</v>
       </c>
-      <c r="E69" s="8" t="s">
+      <c r="E70" s="8" t="s">
         <v>642</v>
       </c>
-      <c r="F69" s="8" t="s">
+      <c r="F70" s="8" t="s">
         <v>641</v>
       </c>
-      <c r="G69">
+      <c r="G70">
         <v>8</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H70" t="s">
         <v>651</v>
       </c>
-      <c r="I69" t="s">
+      <c r="I70" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="238" x14ac:dyDescent="0.2">
-      <c r="A70" s="3">
+    <row r="71" spans="1:11" ht="238" x14ac:dyDescent="0.2">
+      <c r="A71" s="3">
         <v>38113</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>258</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" t="s">
         <v>377</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D71" t="s">
         <v>228</v>
       </c>
-      <c r="E70" s="8" t="s">
+      <c r="E71" s="8" t="s">
         <v>644</v>
       </c>
-      <c r="F70" s="8" t="s">
+      <c r="F71" s="8" t="s">
         <v>643</v>
       </c>
-      <c r="G70">
+      <c r="G71">
         <v>7</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H71" t="s">
         <v>650</v>
       </c>
-      <c r="K70" s="7" t="s">
+      <c r="K71" s="7" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="340" x14ac:dyDescent="0.2">
-      <c r="A71" s="3">
+    <row r="72" spans="1:11" ht="340" x14ac:dyDescent="0.2">
+      <c r="A72" s="3">
         <v>37990</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>260</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C72" t="s">
         <v>381</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D72" t="s">
         <v>351</v>
       </c>
-      <c r="E71" s="8" t="s">
+      <c r="E72" s="8" t="s">
         <v>647</v>
       </c>
-      <c r="F71" s="8" t="s">
+      <c r="F72" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="G71">
+      <c r="G72">
         <v>6</v>
       </c>
-      <c r="H71" t="s">
+      <c r="H72" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="372" x14ac:dyDescent="0.2">
-      <c r="A72" s="3">
+    <row r="73" spans="1:11" ht="372" x14ac:dyDescent="0.2">
+      <c r="A73" s="3">
         <v>37579</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>264</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C73" t="s">
         <v>382</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D73" t="s">
         <v>356</v>
       </c>
-      <c r="E72" s="8" t="s">
+      <c r="E73" s="8" t="s">
         <v>656</v>
       </c>
-      <c r="F72" s="8" t="s">
+      <c r="F73" s="8" t="s">
         <v>657</v>
       </c>
-      <c r="G72">
+      <c r="G73">
         <v>5</v>
       </c>
-      <c r="H72" t="s">
+      <c r="H73" t="s">
         <v>658</v>
       </c>
-      <c r="K72" t="s">
+      <c r="K73" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="272" x14ac:dyDescent="0.2">
-      <c r="A73" s="3">
+    <row r="74" spans="1:11" ht="272" x14ac:dyDescent="0.2">
+      <c r="A74" s="3">
         <v>37494</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B74" t="s">
         <v>268</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C74" t="s">
         <v>383</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D74" t="s">
         <v>228</v>
       </c>
-      <c r="E73" s="8" t="s">
+      <c r="E74" s="8" t="s">
         <v>653</v>
       </c>
-      <c r="F73" s="8" t="s">
+      <c r="F74" s="8" t="s">
         <v>654</v>
       </c>
-      <c r="G73">
+      <c r="G74">
         <v>4</v>
       </c>
-      <c r="H73" s="16" t="s">
+      <c r="H74" s="16" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="356" x14ac:dyDescent="0.2">
-      <c r="A74" s="3">
+    <row r="75" spans="1:11" ht="356" x14ac:dyDescent="0.2">
+      <c r="A75" s="3">
         <v>37208</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>272</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" t="s">
         <v>384</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D75" t="s">
         <v>357</v>
       </c>
-      <c r="E74" s="8" t="s">
+      <c r="E75" s="8" t="s">
         <v>664</v>
       </c>
-      <c r="F74" s="8" t="s">
+      <c r="F75" s="8" t="s">
         <v>665</v>
       </c>
-      <c r="G74">
+      <c r="G75">
         <v>3</v>
       </c>
-      <c r="H74" t="s">
+      <c r="H75" t="s">
         <v>666</v>
       </c>
-      <c r="K74" t="s">
+      <c r="K75" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="272" x14ac:dyDescent="0.2">
-      <c r="A75" s="3">
+    <row r="76" spans="1:11" ht="272" x14ac:dyDescent="0.2">
+      <c r="A76" s="3">
         <v>37107</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
         <v>275</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" t="s">
         <v>385</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D76" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="8" t="s">
+      <c r="E76" s="8" t="s">
         <v>659</v>
       </c>
-      <c r="F75" s="8" t="s">
+      <c r="F76" s="8" t="s">
         <v>661</v>
       </c>
-      <c r="G75">
+      <c r="G76">
         <v>2</v>
       </c>
-      <c r="H75" t="s">
+      <c r="H76" t="s">
         <v>660</v>
       </c>
-      <c r="K75" s="7" t="s">
+      <c r="K76" s="7" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="340" x14ac:dyDescent="0.2">
-      <c r="A76" s="3">
+    <row r="77" spans="1:11" ht="340" x14ac:dyDescent="0.2">
+      <c r="A77" s="3">
         <v>35638</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>278</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C77" t="s">
         <v>386</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D77" t="s">
         <v>277</v>
       </c>
-      <c r="E76" s="8" t="s">
+      <c r="E77" s="8" t="s">
         <v>670</v>
       </c>
-      <c r="F76" s="8" t="s">
+      <c r="F77" s="8" t="s">
         <v>668</v>
       </c>
-      <c r="G76">
+      <c r="G77">
         <v>1</v>
       </c>
-      <c r="H76" t="s">
+      <c r="H77" t="s">
         <v>669</v>
       </c>
-      <c r="I76" t="s">
+      <c r="I77" t="s">
         <v>671</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H14" r:id="rId1" display="http://www.aclweb.org/anthology/P17-1167" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="K14" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="K18" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="I37" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="I38" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="I42" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="I43" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="I46" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="I50" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="I47" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="I48" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="I58" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="I61" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="I62" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="I63" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="I64" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="K75" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="K70" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="K2" r:id="rId19" xr:uid="{6BB7F3D4-BD3A-1D4B-B4ED-D901B7117A9A}"/>
+    <hyperlink ref="H15" r:id="rId1" display="http://www.aclweb.org/anthology/P17-1167" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="K15" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="K19" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="I38" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="I39" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="I43" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="I44" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="I47" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="I51" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="I48" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="I49" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="I59" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="I62" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="I63" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="I64" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="I65" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="K76" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="K71" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="K3" r:id="rId19" xr:uid="{6BB7F3D4-BD3A-1D4B-B4ED-D901B7117A9A}"/>
+    <hyperlink ref="L2" r:id="rId20" xr:uid="{85C9A001-7F74-C342-BC6B-870B1117999E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>